<commit_message>
separated html (class has errors), file attachment, alternative text has own method, variable date/time
</commit_message>
<xml_diff>
--- a/jason.xlsx
+++ b/jason.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jasonxu/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jasonxu/Cue/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,19 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
-  <si>
-    <t>[ ] E120 catch up</t>
-  </si>
-  <si>
-    <t>[ ] Mastering Physics</t>
-  </si>
-  <si>
-    <t>[ ] CS HW</t>
-  </si>
-  <si>
-    <t>[ ] CS Lab</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Tasks</t>
   </si>
@@ -47,22 +35,16 @@
     <t>Due Date</t>
   </si>
   <si>
-    <t>[ ] Clean up iTunes Library</t>
-  </si>
-  <si>
     <t>Friday</t>
   </si>
   <si>
-    <t>unknown</t>
-  </si>
-  <si>
-    <t>Thursday</t>
-  </si>
-  <si>
-    <t>Saturday</t>
-  </si>
-  <si>
-    <t>Monday</t>
+    <t>Related Materials (file name)</t>
+  </si>
+  <si>
+    <t>[ ] CSM</t>
+  </si>
+  <si>
+    <t>week13.pdf</t>
   </si>
 </sst>
 </file>
@@ -385,64 +367,51 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="40.83203125" customWidth="1"/>
+    <col min="3" max="3" width="24.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="1"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="1"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="1"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>